<commit_message>
Change annotation delimiter to double backslash. Because comma is used as delimiter of arguments.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectAnnotationSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A74B2D3-755B-5645-86EA-6E1C4EE2CE6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BDF94A-63AA-E846-A22F-12E8E3929849}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="600" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="500" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -179,29 +179,29 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>Property,Id</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Embedded,Id</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アノテーションのテスト。アノテーションはカンマ区切りで複数記述できます。</t>
-    <rPh sb="27" eb="29">
+    <t>Embedded\\Id</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Property\\Id</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーションのテスト。アノテーションは2重のバックスラッシュ区切りで複数記述できます。</t>
+    <rPh sb="35" eb="37">
       <t>フクスウ</t>
     </rPh>
-    <rPh sb="29" eb="31">
+    <rPh sb="37" eb="39">
       <t>キジュツ</t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>アノテーションのテスト。アノテーションはカンマ区切りで複数記述できます。</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アノテーション付きバリューオブジェクトのサンプル。アノテーションはカンマ区切りで複数記述できます。このクラスは単にサンプルです。実際の動作には利用されません。</t>
+    <t>アノテーションのテスト。アノテーションは2重のバックスラッシュ区切りで複数記述できます。</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーション付きバリューオブジェクトのサンプル。アノテーションは2重のバックスラッシュ区切りで複数記述できます。このクラスは単にサンプルです。実際の動作には利用されません。</t>
     <rPh sb="7" eb="8">
       <t>ツキ</t>
     </rPh>
@@ -690,6 +690,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,15 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,7 +1124,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -1223,12 +1223,12 @@
         <v>2</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="48"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
@@ -1336,41 +1336,41 @@
       <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="42"/>
+      <c r="H19" s="45"/>
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="18"/>
       <c r="J20" s="30"/>
       <c r="K20" s="15"/>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21" t="s">

</xml_diff>

<commit_message>
Now we can specify 'import' command. from now on, Commit generated files also.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BDF94A-63AA-E846-A22F-12E8E3929849}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8B1752-4647-924D-9344-875744EC32BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>クラス名</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>ファイル説明</t>
-  </si>
-  <si>
-    <t>No.</t>
   </si>
   <si>
     <t>フィールド名</t>
@@ -213,12 +210,31 @@
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・インポート</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>xyz.morphia.annotations.*</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>インポートクラス名</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -247,6 +263,13 @@
     <font>
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -283,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -621,11 +644,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -709,6 +812,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1121,10 +1256,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1140,25 +1275,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1172,7 +1307,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1185,7 +1320,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -1194,11 +1329,11 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -1207,11 +1342,11 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -1224,7 +1359,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -1239,7 +1374,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -1248,19 +1383,20 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+    <row r="12" spans="1:11" s="50" customFormat="1">
+      <c r="A12" s="38"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -1290,7 +1426,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
@@ -1301,7 +1437,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1321,179 +1457,264 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="15"/>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A19" s="46" t="s">
+      <c r="A18" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="41"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="65">
+        <v>1</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="41"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="65"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="41"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="66"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="41"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A25" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="C25" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="D25" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="G25" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="45"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="19">
+        <v>1</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="19">
+        <v>2</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="45"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="15"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="19">
-        <v>1</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="15"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="19">
-        <v>2</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="19">
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="19">
         <v>3</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B29" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="19">
+        <v>4</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21" t="s">
+      <c r="F30" s="21"/>
+      <c r="G30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="19">
-        <v>4</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="15"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="G25:H26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F41" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Adapt datetime type as java.util.Date, but not support default value. Adapt default value on php style sheet.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8B1752-4647-924D-9344-875744EC32BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC873989-75DF-0548-A157-F480BD641088}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>クラス名</t>
   </si>
@@ -227,6 +227,10 @@
     <rPh sb="8" eb="9">
       <t>メイ</t>
     </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>"デフォルト"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -793,27 +797,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -844,6 +827,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1259,7 +1263,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1358,12 +1362,12 @@
         <v>2</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
@@ -1383,9 +1387,9 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="1:11" s="50" customFormat="1">
+    <row r="12" spans="1:11" s="43" customFormat="1">
       <c r="A12" s="38"/>
-      <c r="B12" s="49"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
@@ -1466,69 +1470,69 @@
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="G18" s="39"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="35"/>
       <c r="G19" s="40"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
       <c r="K19" s="41"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="65">
+      <c r="A20" s="58">
         <v>1</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
       <c r="K20" s="41"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="65"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
       <c r="K21" s="41"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="66"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
       <c r="K22" s="41"/>
     </row>
     <row r="23" spans="1:11">
@@ -1557,41 +1561,41 @@
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="H25" s="45"/>
+      <c r="H25" s="63"/>
       <c r="I25" s="16"/>
       <c r="J25" s="17"/>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
       <c r="I26" s="18"/>
       <c r="J26" s="30"/>
       <c r="K26" s="15"/>
@@ -1609,7 +1613,7 @@
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G27" s="21" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Adapt createToString and adjustMethodName on PHP type sheet.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectAnnotationSample.xlsx
@@ -8,21 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC873989-75DF-0548-A157-F480BD641088}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC996B5-AFE3-1141-B4F2-8DB588757E02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
+    <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="accessScope">config!$B$4:$B$6</definedName>
+    <definedName name="accessScope2">config!$B$4:$B$5</definedName>
+    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
+    <definedName name="adjustFiledName">config!$H$4:$H$5</definedName>
+    <definedName name="createToString">config!$F$4:$F$5</definedName>
+    <definedName name="isAbstract">config!$D$4:$D$5</definedName>
+    <definedName name="Submit有無" localSheetId="1">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
+    <definedName name="toString">config!$F$4:$F$5</definedName>
+    <definedName name="Validate実装パターン" localSheetId="1">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
+    <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
+    <definedName name="デリミタ" localSheetId="1">#REF!</definedName>
     <definedName name="デリミタ">#REF!</definedName>
+    <definedName name="デリミタ選択肢" localSheetId="1">#REF!</definedName>
     <definedName name="デリミタ選択肢">#REF!</definedName>
+    <definedName name="型" localSheetId="1">#REF!</definedName>
     <definedName name="型">#REF!</definedName>
+    <definedName name="項目型" localSheetId="1">#REF!</definedName>
     <definedName name="項目型">#REF!</definedName>
+    <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
@@ -43,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>クラス名</t>
   </si>
@@ -233,12 +252,77 @@
     <t>"デフォルト"</t>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>バリューオブジェクト定義書 設定シート</t>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>様式 ver 0.9.9 (2007.12.06)</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>アクセス</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>抽象クラス</t>
+    <rPh sb="0" eb="2">
+      <t>チュウショウ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>toStringメソッド</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>フィールド名の変形</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヘンケイ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>デフォルト値の変形</t>
+    <rPh sb="7" eb="9">
+      <t>ヘンケイ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>public</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>toStringメソッドの生成</t>
+    <rPh sb="13" eb="15">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>フィールド名の変形</t>
+    <phoneticPr fontId="7"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -277,8 +361,20 @@
       <family val="2"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,8 +405,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -728,11 +830,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -850,9 +1020,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{C23F3EF4-69BC-7141-8411-546FCAC88B19}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -933,6 +1134,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="valueObject"/>
+      <sheetName val="config"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1260,10 +1476,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1387,148 +1603,148 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
     </row>
-    <row r="12" spans="1:11" s="43" customFormat="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="31" t="s">
+    <row r="12" spans="1:11" s="33" customFormat="1">
+      <c r="A12" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:11" s="33" customFormat="1">
+      <c r="A13" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="77"/>
+      <c r="C13" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:11" s="43" customFormat="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="34" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="3" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="31" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="54" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B21" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="41"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="58">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="41"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="58">
         <v>1</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B22" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="41"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="58"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="41"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="59"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="52"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
@@ -1536,156 +1752,136 @@
       <c r="K22" s="41"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="41"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="41"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A25" s="64" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A27" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B27" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C27" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="D27" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E27" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="63" t="s">
+      <c r="F27" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="63" t="s">
+      <c r="G27" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="H25" s="63"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="64"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="19">
-        <v>1</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="15"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="19">
-        <v>2</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="30"/>
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D29" s="21"/>
-      <c r="E29" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="G29" s="21" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
-      <c r="J29" s="23"/>
+      <c r="J29" s="29"/>
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21" t="s">
-        <v>32</v>
-      </c>
+      <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -1693,34 +1889,86 @@
       <c r="K30" s="15"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="28"/>
+      <c r="A31" s="19">
+        <v>3</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="23"/>
       <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="19">
+        <v>4</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G25:H26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="G27:H28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F47" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F49" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+      <formula1>adjustFiledName</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
+      <formula1>createToString</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
@@ -1729,4 +1977,98 @@
     <oddFooter>&amp;C&amp;P / &amp;N ページ&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28F8D6F-DFFA-2242-9EC0-DE0C421F719A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="69" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="69" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="69" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="69" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="11" max="256" width="8.83203125" style="69" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="69"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="19">
+      <c r="A1" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="68"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="J4" s="72"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="75"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>